<commit_message>
Doing real analysis now
</commit_message>
<xml_diff>
--- a/data/LL97Parameters .xlsx
+++ b/data/LL97Parameters .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulr\Documents\R\cbwg\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD19048E-984D-4E4E-9160-63C937A58693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B159F5-8FA1-40F7-8719-9886F9477053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10882" yWindow="3945" windowWidth="9638" windowHeight="8003" activeTab="1" xr2:uid="{D1FF0304-57B1-418A-BA32-60C9B26F52A1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{D1FF0304-57B1-418A-BA32-60C9B26F52A1}"/>
   </bookViews>
   <sheets>
     <sheet name="EmissionsLimits" sheetId="2" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>Energy</t>
   </si>
   <si>
-    <t>Electric</t>
-  </si>
-  <si>
     <t>N.Gas</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>Period</t>
+  </si>
+  <si>
+    <t>Elect</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -919,7 +919,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -940,12 +940,12 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>2.8896199999999998E-4</v>
@@ -959,13 +959,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>5.3109999999999998E-5</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>2024</v>
@@ -973,13 +973,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>7.4209999999999996E-5</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>2024</v>
@@ -987,13 +987,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>7.5290000000000006E-5</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>2024</v>
@@ -1001,13 +1001,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>4.4929999999999998E-5</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>2024</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>